<commit_message>
Run for NLP job. Into user test stage
</commit_message>
<xml_diff>
--- a/Excel_file/test.xlsx
+++ b/Excel_file/test.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k25063738/Named_entity_algorithm_project/Excel_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BF32BD6-105E-8D46-A93C-55F16D89EAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CD2B6F8-3248-5642-A0CD-F82CB95AFD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20780" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{658919FD-496C-3C47-BE31-5EFDA43CCB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2912,10 +2913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E29079E-5F27-004B-81ED-5DF464220C18}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BT80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD80"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>